<commit_message>
Update .gitignore, modify database password, enhance JSP files with JSTL tags, and remove unused SendEmail class
</commit_message>
<xml_diff>
--- a/web/WEB-INF/Excel/Assignment/Reading/Starter_TOEIC_ReadingUnit1.xlsx
+++ b/web/WEB-INF/Excel/Assignment/Reading/Starter_TOEIC_ReadingUnit1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GITPRJ\PRJ301_LearningApp\excel\Assignment\Reading\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GITPRJ\PRJ301_LearningApp\web\WEB-INF\Excel\Assignment\Reading\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1E64BCE-4CE4-4E3D-B10D-FBE273567CEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B49C740B-5FAA-4D0E-A64D-555783C7ED83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1464" yWindow="1464" windowWidth="12768" windowHeight="8880" xr2:uid="{EBCB4850-619C-430F-974B-9AFB0CA94A59}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{EBCB4850-619C-430F-974B-9AFB0CA94A59}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,8 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -398,7 +396,7 @@
     <t>What did he ...... her to do this morning?</t>
   </si>
   <si>
-    <t>Mr. Albert Di Beni, / 333 Spring Road / Penshurst/ Kent / Dear Mr.Di beni, / The Penshurst Medical Practice invites you to make an appointment for a medical (...1...). / After the age of forty, we recommend that you have a full physical every year. Our records show that you recently(…2…) your fiftieth birthday. However, it is over seven years since/your last appointment with our clinic. If you contact the Penshurst Medical Practice before September 15th, you will be able to take advantage (....3...) a free check up. In this medical / we will check blood pressure, blood cholesterol, and blood sugar. For a small extra charge, it is possible to have a more detailed examination. If you are (...4...) in this offer, please call / the Medical Practice at your earliest   convenience./ Sincerely, / Penshurst Medical Practice / It is important to stretch both before and after exercising. Many fitness experts say that stretching after you exercise is actually more important than before. However, many people do not bother stretching after their workout. They say that they are too (...5...), or they just / forget. Stretching has many benefits. For example, it helps you avoid painful cramps in your muscles. If you don't stretch, you could have tight and sore muscles the next day. It helps to (....6…)your flexibility. If you stretch after every workout, it will be easy to touch your toes. / You might be surprised to know how many people(....7...) reach their toes. Finally, it is also a / good way to relax and wind down after strenuous exercise. So be sure to(...8...) ten minutes / Red Cross December Blood Drive / The Red Cross (...9...) like to thank its regular donors for all their contributions. Without / your help, we could not continue with our good work. Every pint of blood that you donate allows us to help people in need. Your blood saves lives. Our next blood drive will(....10...) on / December 22nd, from 9 a.m. to 7 p.m. It will be held at the Red Cross Hall on Lion Street. We are staying open later than(...11...) so that working people can drop by after work. If you have / donated before, please bring your registration card to save time. First time donors are also more than welcome. Please encourage your friends and family members to come along, too. Giving up less than one hour of their time could give many more years of life to another(...12...)</t>
+    <t>Mr. Albert Di Beni, / 333 Spring Road / Penshurst/ Kent / Dear Mr.Di beni, / The Penshurst Medical Practice invites you to make an appointment for a medical (...1...).  After the age of forty, we recommend that you have a full physical every year. Our records show that you recently(…2…) your fiftieth birthday. However, it is over seven years since your last appointment with our clinic. If you contact the Penshurst Medical Practice before September 15th, you will be able to take advantage (....3...) a free check up. In this medical  we will check blood pressure, blood cholesterol, and blood sugar. For a small extra charge, it is possible to have a more detailed examination. If you are (...4...) in this offer, please call  the Medical Practice at your earliest   convenience./ Sincerely, / Penshurst Medical Practice / It is important to stretch both before and after exercising. Many fitness experts say that stretching after you exercise is actually more important than before. However, many people do not bother stretching after their workout. They say that they are too (...5...), or they just  forget. Stretching has many benefits. For example, it helps you avoid painful cramps in your muscles. If you don't stretch, you could have tight and sore muscles the next day. It helps to (....6…)your flexibility. If you stretch after every workout, it will be easy to touch your toes.  You might be surprised to know how many people(....7...) reach their toes. Finally, it is also a  good way to relax and wind down after strenuous exercise. So be sure to(...8...) ten minutes  Red Cross December Blood Drive  The Red Cross (...9...) like to thank its regular donors for all their contributions. Without  your help, we could not continue with our good work. Every pint of blood that you donate allows us to help people in need. Your blood saves lives. Our next blood drive will(....10...) on  December 22nd, from 9 a.m. to 7 p.m. It will be held at the Red Cross Hall on Lion Street. We are staying open later than(...11...) so that working people can drop by after work. If you have  donated before, please bring your registration card to save time. First time donors are also more than welcome. Please encourage your friends and family members to come along, too. Giving up less than one hour of their time could give many more years of life to another(...12...)</t>
   </si>
 </sst>
 </file>
@@ -801,8 +799,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F050C06-3D01-4598-8B25-B8D083FE07B6}">
   <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>